<commit_message>
top goal scorers and palyer nation vs goal scored analysis done
</commit_message>
<xml_diff>
--- a/Data Sources/ChampionsLeague.xlsx
+++ b/Data Sources/ChampionsLeague.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCL23-24_analytics\Data Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9530DA7F-2D05-4BB2-B86B-0A51A7D9AE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="23-24 Season" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="130">
   <si>
     <t>Rk</t>
   </si>
@@ -72,9 +73,6 @@
     <t>Top Team Scorer</t>
   </si>
   <si>
-    <t>Goalkeeper</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -87,12 +85,6 @@
     <t>W W W W D</t>
   </si>
   <si>
-    <t>Joselu, Vinicius Júnior... - 5</t>
-  </si>
-  <si>
-    <t>Andriy Lunin</t>
-  </si>
-  <si>
     <t>es</t>
   </si>
   <si>
@@ -102,12 +94,6 @@
     <t>W W W L W</t>
   </si>
   <si>
-    <t>Niclas Füllkrug - 3</t>
-  </si>
-  <si>
-    <t>Gregor Kobel</t>
-  </si>
-  <si>
     <t>de</t>
   </si>
   <si>
@@ -120,24 +106,12 @@
     <t>D L L W L</t>
   </si>
   <si>
-    <t>Harry Kane - 8</t>
-  </si>
-  <si>
-    <t>Manuel Neuer</t>
-  </si>
-  <si>
     <t>Paris S-G</t>
   </si>
   <si>
     <t>L L L W W</t>
   </si>
   <si>
-    <t>Kylian Mbappé - 8</t>
-  </si>
-  <si>
-    <t>Gianluigi Donnarumma</t>
-  </si>
-  <si>
     <t>fr</t>
   </si>
   <si>
@@ -150,12 +124,6 @@
     <t>W W W W W</t>
   </si>
   <si>
-    <t>Erling Haaland - 6</t>
-  </si>
-  <si>
-    <t>Ederson</t>
-  </si>
-  <si>
     <t>eng</t>
   </si>
   <si>
@@ -165,33 +133,15 @@
     <t>W W W W L</t>
   </si>
   <si>
-    <t>Antoine Griezmann - 6</t>
-  </si>
-  <si>
-    <t>Jan Oblak</t>
-  </si>
-  <si>
     <t>Barcelona</t>
   </si>
   <si>
     <t>W L W W W</t>
   </si>
   <si>
-    <t>Robert Lewandowski, Ferrán Torres... - 3</t>
-  </si>
-  <si>
-    <t>Marc-André ter Stegen</t>
-  </si>
-  <si>
     <t>Arsenal</t>
   </si>
   <si>
-    <t>Leandro Trossard, Gabriel Jesus... - 4</t>
-  </si>
-  <si>
-    <t>David Raya</t>
-  </si>
-  <si>
     <t>R16</t>
   </si>
   <si>
@@ -201,12 +151,6 @@
     <t>W D W W W</t>
   </si>
   <si>
-    <t>Galeno - 5</t>
-  </si>
-  <si>
-    <t>Diogo Costa</t>
-  </si>
-  <si>
     <t>pt</t>
   </si>
   <si>
@@ -216,12 +160,6 @@
     <t>W W L W D</t>
   </si>
   <si>
-    <t>Alexis Sánchez, Marko Arnautović... - 2</t>
-  </si>
-  <si>
-    <t>Yann Sommer</t>
-  </si>
-  <si>
     <t>it</t>
   </si>
   <si>
@@ -231,60 +169,30 @@
     <t>W W D D D</t>
   </si>
   <si>
-    <t>Loïs Openda - 4</t>
-  </si>
-  <si>
-    <t>Janis Blaswich</t>
-  </si>
-  <si>
     <t>Lazio</t>
   </si>
   <si>
     <t>W W D W D</t>
   </si>
   <si>
-    <t>Ciro Immobile - 4</t>
-  </si>
-  <si>
-    <t>Ivan Provedel</t>
-  </si>
-  <si>
     <t>Real Sociedad</t>
   </si>
   <si>
     <t>L W L W W</t>
   </si>
   <si>
-    <t>Brais Méndez - 3</t>
-  </si>
-  <si>
-    <t>Álex Remiro</t>
-  </si>
-  <si>
     <t>Napoli</t>
   </si>
   <si>
     <t>L D D L D</t>
   </si>
   <si>
-    <t>Victor Osimhen - 2</t>
-  </si>
-  <si>
-    <t>Alex Meret</t>
-  </si>
-  <si>
     <t>PSV Eindhoven</t>
   </si>
   <si>
     <t>W W W D W</t>
   </si>
   <si>
-    <t>Luuk de Jong - 3</t>
-  </si>
-  <si>
-    <t>Walter Benítez</t>
-  </si>
-  <si>
     <t>nl</t>
   </si>
   <si>
@@ -294,12 +202,6 @@
     <t>W W W L L</t>
   </si>
   <si>
-    <t>Mohamed Elyounoussi, Lukas Lerager - 3</t>
-  </si>
-  <si>
-    <t>Kamil Grabara</t>
-  </si>
-  <si>
     <t>dk</t>
   </si>
   <si>
@@ -309,12 +211,6 @@
     <t>Shakhtar</t>
   </si>
   <si>
-    <t>Danylo Sikan - 4</t>
-  </si>
-  <si>
-    <t>Dmytro Riznyk</t>
-  </si>
-  <si>
     <t>ua</t>
   </si>
   <si>
@@ -324,54 +220,24 @@
     <t>L D D W L</t>
   </si>
   <si>
-    <t>Samuel Chukwueze - 2</t>
-  </si>
-  <si>
-    <t>Mike Maignan</t>
-  </si>
-  <si>
     <t>Lens</t>
   </si>
   <si>
     <t>W L W D D</t>
   </si>
   <si>
-    <t>Angelo Fulgini, Elye Wahi - 2</t>
-  </si>
-  <si>
-    <t>Brice Samba</t>
-  </si>
-  <si>
     <t>Feyenoord</t>
   </si>
   <si>
-    <t>Santiago Giménez - 2</t>
-  </si>
-  <si>
-    <t>Justin Bijlow</t>
-  </si>
-  <si>
     <t>Newcastle Utd</t>
   </si>
   <si>
     <t>W W D L W</t>
   </si>
   <si>
-    <t>Dan Burn, Fabian Schär... - 1</t>
-  </si>
-  <si>
-    <t>Nick Pope</t>
-  </si>
-  <si>
     <t>Galatasaray</t>
   </si>
   <si>
-    <t>Mauro Icardi, Hakim Ziyech... - 2</t>
-  </si>
-  <si>
-    <t>Fernando Muslera</t>
-  </si>
-  <si>
     <t>tr</t>
   </si>
   <si>
@@ -381,33 +247,15 @@
     <t>D L L W W</t>
   </si>
   <si>
-    <t>Rasmus Højlund - 5</t>
-  </si>
-  <si>
-    <t>André Onana</t>
-  </si>
-  <si>
     <t>Benfica</t>
   </si>
   <si>
-    <t>João Mário - 3</t>
-  </si>
-  <si>
-    <t>Anatolii Trubin</t>
-  </si>
-  <si>
     <t>RB Salzburg</t>
   </si>
   <si>
     <t>L D L W W</t>
   </si>
   <si>
-    <t>Oscar Gloukh - 2</t>
-  </si>
-  <si>
-    <t>Alexander Schlager</t>
-  </si>
-  <si>
     <t>at</t>
   </si>
   <si>
@@ -417,12 +265,6 @@
     <t>W W L W W</t>
   </si>
   <si>
-    <t>Meschak Elia - 2</t>
-  </si>
-  <si>
-    <t>Anthony Racioppi</t>
-  </si>
-  <si>
     <t>ch</t>
   </si>
   <si>
@@ -432,21 +274,9 @@
     <t>W L W W L</t>
   </si>
   <si>
-    <t>Bruma, Álvaro djaló - 2</t>
-  </si>
-  <si>
-    <t>Matheus</t>
-  </si>
-  <si>
     <t>Celtic</t>
   </si>
   <si>
-    <t>Kyogo Furuhashi, Luis Enrique Palma - 2</t>
-  </si>
-  <si>
-    <t>Joe Hart</t>
-  </si>
-  <si>
     <t>sct</t>
   </si>
   <si>
@@ -456,12 +286,6 @@
     <t>L L L L L</t>
   </si>
   <si>
-    <t>Vincent Janssen, Arbnor Muja... - 1</t>
-  </si>
-  <si>
-    <t>Jean Butez</t>
-  </si>
-  <si>
     <t>be</t>
   </si>
   <si>
@@ -471,46 +295,127 @@
     <t>L D L L W</t>
   </si>
   <si>
-    <t>Sheraldo Becker - 2</t>
-  </si>
-  <si>
-    <t>Frederik Rønnow</t>
-  </si>
-  <si>
     <t>Sevilla</t>
   </si>
   <si>
     <t>D W L L L</t>
   </si>
   <si>
-    <t>Sergio Ramos, Nemanja Gudelj... - 2</t>
-  </si>
-  <si>
-    <t>Marko Dmitrović</t>
-  </si>
-  <si>
     <t>Red Star</t>
   </si>
   <si>
     <t>D W W W W</t>
   </si>
   <si>
-    <t>Osman Bukari - 2</t>
-  </si>
-  <si>
-    <t>Omri Glazer</t>
-  </si>
-  <si>
     <t>rs</t>
   </si>
   <si>
     <t>S.N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joselu, Vinicius Júnior... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niclas Füllkrug </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harry Kane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kylian Mbappé </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erling Haaland </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antoine Griezmann </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert Lewandowski, Ferrán Torres... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leandro Trossard, Gabriel Jesus... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galeno </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexis Sánchez, Marko Arnautović... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loïs Openda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciro Immobile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brais Méndez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victor Osimhen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luuk de Jong </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohamed Elyounoussi, Lukas Lerager </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danylo Sikan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samuel Chukwueze </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angelo Fulgini, Elye Wahi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santiago Giménez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dan Burn, Fabian Schär... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauro Icardi, Hakim Ziyech... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rasmus Højlund </t>
+  </si>
+  <si>
+    <t xml:space="preserve">João Mário </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oscar Gloukh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meschak Elia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bruma, Álvaro djaló </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyogo Furuhashi, Luis Enrique Palma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vincent Janssen, Arbnor Muja... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheraldo Becker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sergio Ramos, Nemanja Gudelj... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osman Bukari </t>
+  </si>
+  <si>
+    <t>Goals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -875,18 +780,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>161</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -940,21 +865,21 @@
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
       </c>
       <c r="D2">
         <v>12</v>
@@ -993,30 +918,30 @@
         <v>0.72</v>
       </c>
       <c r="P2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q2">
         <v>72777</v>
       </c>
       <c r="R2" t="s">
+        <v>97</v>
+      </c>
+      <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
-      </c>
-      <c r="S2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
       <c r="D3">
         <v>12</v>
@@ -1055,30 +980,30 @@
         <v>-0.61</v>
       </c>
       <c r="P3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="Q3">
         <v>81365</v>
       </c>
       <c r="R3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" t="s">
-        <v>28</v>
+        <v>98</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
       </c>
       <c r="T3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>12</v>
@@ -1117,30 +1042,30 @@
         <v>0.33</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="Q4">
         <v>75000</v>
       </c>
       <c r="R4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" t="s">
-        <v>34</v>
+        <v>99</v>
+      </c>
+      <c r="S4">
+        <v>8</v>
       </c>
       <c r="T4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>12</v>
@@ -1179,30 +1104,30 @@
         <v>0.91</v>
       </c>
       <c r="P5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="Q5">
         <v>46686</v>
       </c>
       <c r="R5" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" t="s">
-        <v>38</v>
+        <v>100</v>
+      </c>
+      <c r="S5">
+        <v>8</v>
       </c>
       <c r="T5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1241,30 +1166,30 @@
         <v>1.77</v>
       </c>
       <c r="P6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="Q6">
         <v>51298</v>
       </c>
       <c r="R6" t="s">
-        <v>43</v>
-      </c>
-      <c r="S6" t="s">
-        <v>44</v>
+        <v>101</v>
+      </c>
+      <c r="S6">
+        <v>6</v>
       </c>
       <c r="T6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -1303,30 +1228,30 @@
         <v>0.39</v>
       </c>
       <c r="P7" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q7">
         <v>64803</v>
       </c>
       <c r="R7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S7" t="s">
-        <v>49</v>
+        <v>102</v>
+      </c>
+      <c r="S7">
+        <v>6</v>
       </c>
       <c r="T7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -1365,30 +1290,30 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="P8" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="Q8">
         <v>45308</v>
       </c>
       <c r="R8" t="s">
-        <v>52</v>
-      </c>
-      <c r="S8" t="s">
-        <v>53</v>
+        <v>103</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
       </c>
       <c r="T8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -1427,30 +1352,30 @@
         <v>0.49</v>
       </c>
       <c r="P9" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="Q9">
         <v>59870</v>
       </c>
       <c r="R9" t="s">
-        <v>55</v>
-      </c>
-      <c r="S9" t="s">
-        <v>56</v>
+        <v>104</v>
+      </c>
+      <c r="S9">
+        <v>4</v>
       </c>
       <c r="T9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -1489,30 +1414,30 @@
         <v>0.46</v>
       </c>
       <c r="P10" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="Q10">
         <v>47944</v>
       </c>
       <c r="R10" t="s">
-        <v>60</v>
-      </c>
-      <c r="S10" t="s">
-        <v>61</v>
+        <v>105</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
       </c>
       <c r="T10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -1551,30 +1476,30 @@
         <v>0.94</v>
       </c>
       <c r="P11" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="Q11">
         <v>70279</v>
       </c>
       <c r="R11" t="s">
-        <v>65</v>
-      </c>
-      <c r="S11" t="s">
-        <v>66</v>
+        <v>106</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
       </c>
       <c r="T11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -1613,30 +1538,30 @@
         <v>0.19</v>
       </c>
       <c r="P12" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="Q12">
         <v>43949</v>
       </c>
       <c r="R12" t="s">
-        <v>70</v>
-      </c>
-      <c r="S12" t="s">
-        <v>71</v>
+        <v>107</v>
+      </c>
+      <c r="S12">
+        <v>4</v>
       </c>
       <c r="T12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -1675,30 +1600,30 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="P13" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="Q13">
         <v>47701</v>
       </c>
       <c r="R13" t="s">
-        <v>74</v>
-      </c>
-      <c r="S13" t="s">
-        <v>75</v>
+        <v>108</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
       </c>
       <c r="T13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>8</v>
@@ -1737,30 +1662,30 @@
         <v>0.49</v>
       </c>
       <c r="P14" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="Q14">
         <v>36790</v>
       </c>
       <c r="R14" t="s">
-        <v>78</v>
-      </c>
-      <c r="S14" t="s">
-        <v>79</v>
+        <v>109</v>
+      </c>
+      <c r="S14">
+        <v>3</v>
       </c>
       <c r="T14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>8</v>
@@ -1799,30 +1724,30 @@
         <v>-0.13</v>
       </c>
       <c r="P15" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="Q15">
         <v>45367</v>
       </c>
       <c r="R15" t="s">
-        <v>82</v>
-      </c>
-      <c r="S15" t="s">
-        <v>83</v>
+        <v>110</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
       </c>
       <c r="T15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="D16">
         <v>8</v>
@@ -1861,30 +1786,30 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="Q16">
         <v>34589</v>
       </c>
       <c r="R16" t="s">
-        <v>86</v>
-      </c>
-      <c r="S16" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="S16">
+        <v>3</v>
       </c>
       <c r="T16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="D17">
         <v>8</v>
@@ -1923,30 +1848,30 @@
         <v>-0.46</v>
       </c>
       <c r="P17" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="Q17">
         <v>35592</v>
       </c>
       <c r="R17" t="s">
-        <v>91</v>
-      </c>
-      <c r="S17" t="s">
-        <v>92</v>
+        <v>112</v>
+      </c>
+      <c r="S17">
+        <v>3</v>
       </c>
       <c r="T17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -1985,30 +1910,30 @@
         <v>-0.57999999999999996</v>
       </c>
       <c r="P18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q18">
         <v>47695</v>
       </c>
       <c r="R18" t="s">
-        <v>96</v>
-      </c>
-      <c r="S18" t="s">
-        <v>97</v>
+        <v>113</v>
+      </c>
+      <c r="S18">
+        <v>4</v>
       </c>
       <c r="T18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="D19">
         <v>6</v>
@@ -2047,30 +1972,30 @@
         <v>0.32</v>
       </c>
       <c r="P19" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="Q19">
         <v>72212</v>
       </c>
       <c r="R19" t="s">
-        <v>101</v>
-      </c>
-      <c r="S19" t="s">
-        <v>102</v>
+        <v>114</v>
+      </c>
+      <c r="S19">
+        <v>2</v>
       </c>
       <c r="T19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="D20">
         <v>6</v>
@@ -2109,30 +2034,30 @@
         <v>-0.23</v>
       </c>
       <c r="P20" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="Q20">
         <v>37543</v>
       </c>
       <c r="R20" t="s">
-        <v>105</v>
-      </c>
-      <c r="S20" t="s">
-        <v>106</v>
+        <v>115</v>
+      </c>
+      <c r="S20">
+        <v>2</v>
       </c>
       <c r="T20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -2171,30 +2096,30 @@
         <v>0.43</v>
       </c>
       <c r="P21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="Q21">
         <v>44010</v>
       </c>
       <c r="R21" t="s">
-        <v>108</v>
-      </c>
-      <c r="S21" t="s">
-        <v>109</v>
+        <v>116</v>
+      </c>
+      <c r="S21">
+        <v>2</v>
       </c>
       <c r="T21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="D22">
         <v>6</v>
@@ -2233,30 +2158,30 @@
         <v>-1.07</v>
       </c>
       <c r="P22" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="Q22">
         <v>52023</v>
       </c>
       <c r="R22" t="s">
-        <v>112</v>
-      </c>
-      <c r="S22" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
       </c>
       <c r="T22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="D23">
         <v>6</v>
@@ -2295,30 +2220,30 @@
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="P23" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="Q23">
         <v>50140</v>
       </c>
       <c r="R23" t="s">
-        <v>115</v>
-      </c>
-      <c r="S23" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="S23">
+        <v>2</v>
       </c>
       <c r="T23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -2357,30 +2282,30 @@
         <v>-0.15</v>
       </c>
       <c r="P24" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="Q24">
         <v>73175</v>
       </c>
       <c r="R24" t="s">
-        <v>120</v>
-      </c>
-      <c r="S24" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="S24">
+        <v>5</v>
       </c>
       <c r="T24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="D25">
         <v>6</v>
@@ -2419,30 +2344,30 @@
         <v>-1.34</v>
       </c>
       <c r="P25" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="Q25">
         <v>56621</v>
       </c>
       <c r="R25" t="s">
-        <v>123</v>
-      </c>
-      <c r="S25" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="S25">
+        <v>3</v>
       </c>
       <c r="T25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="D26">
         <v>6</v>
@@ -2481,30 +2406,30 @@
         <v>-0.66</v>
       </c>
       <c r="P26" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="Q26">
         <v>28477</v>
       </c>
       <c r="R26" t="s">
-        <v>127</v>
-      </c>
-      <c r="S26" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="S26">
+        <v>2</v>
       </c>
       <c r="T26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="D27">
         <v>6</v>
@@ -2543,30 +2468,30 @@
         <v>-1.48</v>
       </c>
       <c r="P27" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="Q27">
         <v>31500</v>
       </c>
       <c r="R27" t="s">
-        <v>132</v>
-      </c>
-      <c r="S27" t="s">
-        <v>133</v>
+        <v>122</v>
+      </c>
+      <c r="S27">
+        <v>2</v>
       </c>
       <c r="T27" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="D28">
         <v>6</v>
@@ -2605,30 +2530,30 @@
         <v>-0.28000000000000003</v>
       </c>
       <c r="P28" t="s">
-        <v>136</v>
+        <v>83</v>
       </c>
       <c r="Q28">
         <v>21366</v>
       </c>
       <c r="R28" t="s">
-        <v>137</v>
-      </c>
-      <c r="S28" t="s">
-        <v>138</v>
+        <v>123</v>
+      </c>
+      <c r="S28">
+        <v>2</v>
       </c>
       <c r="T28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>139</v>
+        <v>84</v>
       </c>
       <c r="D29">
         <v>6</v>
@@ -2667,30 +2592,30 @@
         <v>-1.1299999999999999</v>
       </c>
       <c r="P29" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="Q29">
         <v>56099</v>
       </c>
       <c r="R29" t="s">
-        <v>140</v>
-      </c>
-      <c r="S29" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="S29">
+        <v>2</v>
       </c>
       <c r="T29" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>86</v>
       </c>
       <c r="D30">
         <v>6</v>
@@ -2729,30 +2654,30 @@
         <v>-0.81</v>
       </c>
       <c r="P30" t="s">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="Q30">
         <v>13570</v>
       </c>
       <c r="R30" t="s">
-        <v>145</v>
-      </c>
-      <c r="S30" t="s">
-        <v>146</v>
+        <v>125</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
       </c>
       <c r="T30" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
+        <v>89</v>
       </c>
       <c r="D31">
         <v>6</v>
@@ -2791,30 +2716,30 @@
         <v>-0.98</v>
       </c>
       <c r="P31" t="s">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="Q31">
         <v>72976</v>
       </c>
       <c r="R31" t="s">
-        <v>150</v>
-      </c>
-      <c r="S31" t="s">
-        <v>151</v>
+        <v>126</v>
+      </c>
+      <c r="S31">
+        <v>2</v>
       </c>
       <c r="T31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -2853,30 +2778,30 @@
         <v>-0.81</v>
       </c>
       <c r="P32" t="s">
-        <v>153</v>
+        <v>92</v>
       </c>
       <c r="Q32">
         <v>34181</v>
       </c>
       <c r="R32" t="s">
-        <v>154</v>
-      </c>
-      <c r="S32" t="s">
-        <v>155</v>
+        <v>127</v>
+      </c>
+      <c r="S32">
+        <v>2</v>
       </c>
       <c r="T32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>93</v>
       </c>
       <c r="D33">
         <v>6</v>
@@ -2915,25 +2840,25 @@
         <v>-1.02</v>
       </c>
       <c r="P33" t="s">
-        <v>157</v>
+        <v>94</v>
       </c>
       <c r="Q33">
         <v>46202</v>
       </c>
       <c r="R33" t="s">
-        <v>158</v>
-      </c>
-      <c r="S33" t="s">
-        <v>159</v>
+        <v>128</v>
+      </c>
+      <c r="S33">
+        <v>2</v>
       </c>
       <c r="T33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
     </row>
   </sheetData>

</xml_diff>